<commit_message>
Updated EDA notebook, Taxes data
Updated EDA notebook analysis, used a different version of Taxes data
</commit_message>
<xml_diff>
--- a/DATA/TAXES.xlsx
+++ b/DATA/TAXES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrew\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/synikola/Desktop/Github/EDAChallenge2022/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4F449B-95B0-44C4-9EF7-CC5C2C45DCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513E0A64-6316-A944-99C4-CF75DEAB169B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{04ABF146-0EDD-C644-BFA3-7D76600FDCE1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{04ABF146-0EDD-C644-BFA3-7D76600FDCE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="155">
   <si>
     <t>State</t>
   </si>
@@ -496,162 +496,6 @@
   </si>
   <si>
     <t>DC</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>Alabama, AL</t>
-  </si>
-  <si>
-    <t>Alaska, AK</t>
-  </si>
-  <si>
-    <t>Arizona, AZ</t>
-  </si>
-  <si>
-    <t>Arkansas, AR</t>
-  </si>
-  <si>
-    <t>California, CA</t>
-  </si>
-  <si>
-    <t>Colorado, CO</t>
-  </si>
-  <si>
-    <t>Connecticut, CT</t>
-  </si>
-  <si>
-    <t>Delaware, DE</t>
-  </si>
-  <si>
-    <t>District of Columbia, DC</t>
-  </si>
-  <si>
-    <t>Florida, FL</t>
-  </si>
-  <si>
-    <t>Georgia, GA</t>
-  </si>
-  <si>
-    <t>Hawaii, HI</t>
-  </si>
-  <si>
-    <t>Idaho, ID</t>
-  </si>
-  <si>
-    <t>Illinois, IL</t>
-  </si>
-  <si>
-    <t>Indiana, IN</t>
-  </si>
-  <si>
-    <t>Iowa, IA</t>
-  </si>
-  <si>
-    <t>Kansas, KS</t>
-  </si>
-  <si>
-    <t>Kentucky, KY</t>
-  </si>
-  <si>
-    <t>Louisiana, LA</t>
-  </si>
-  <si>
-    <t>Maine, ME</t>
-  </si>
-  <si>
-    <t>Maryland, MD</t>
-  </si>
-  <si>
-    <t>Massachusetts, MA</t>
-  </si>
-  <si>
-    <t>Michigan, MI</t>
-  </si>
-  <si>
-    <t>Minnesota, MN</t>
-  </si>
-  <si>
-    <t>Mississippi, MS</t>
-  </si>
-  <si>
-    <t>Missouri, MO</t>
-  </si>
-  <si>
-    <t>Montana, MT</t>
-  </si>
-  <si>
-    <t>Nebraska, NE</t>
-  </si>
-  <si>
-    <t>Nevada, NV</t>
-  </si>
-  <si>
-    <t>New Hampshire, NH</t>
-  </si>
-  <si>
-    <t>New Jersey, NJ</t>
-  </si>
-  <si>
-    <t>New Mexico, NM</t>
-  </si>
-  <si>
-    <t>New York, NY</t>
-  </si>
-  <si>
-    <t>North Carolina, NC</t>
-  </si>
-  <si>
-    <t>North Dakota, ND</t>
-  </si>
-  <si>
-    <t>Ohio, OH</t>
-  </si>
-  <si>
-    <t>Oklahoma, OK</t>
-  </si>
-  <si>
-    <t>Oregon, OR</t>
-  </si>
-  <si>
-    <t>Pennsylvania, PA</t>
-  </si>
-  <si>
-    <t>Rhode Island, RI</t>
-  </si>
-  <si>
-    <t>South Carolina, SC</t>
-  </si>
-  <si>
-    <t>South Dakota, SD</t>
-  </si>
-  <si>
-    <t>Tennessee, TN</t>
-  </si>
-  <si>
-    <t>Texas, TX</t>
-  </si>
-  <si>
-    <t>Utah, UT</t>
-  </si>
-  <si>
-    <t>Vermont, VT</t>
-  </si>
-  <si>
-    <t>Virginia, VA</t>
-  </si>
-  <si>
-    <t>Washington, WA</t>
-  </si>
-  <si>
-    <t>West Virginia, WV</t>
-  </si>
-  <si>
-    <t>Wisconsin, WI</t>
-  </si>
-  <si>
-    <t>Wyoming, WY</t>
   </si>
   <si>
     <t>State HEADLINES</t>
@@ -1020,744 +864,588 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{027FCBB9-133E-7E4F-8C3C-CD89F2423E7A}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D52"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="37.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="37.125" customWidth="1"/>
-    <col min="4" max="4" width="34.5" customWidth="1"/>
+    <col min="1" max="1" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21.75">
+    <row r="1" spans="1:3" ht="22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>206</v>
+        <v>154</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="22.5">
+    <row r="2" spans="1:3" ht="23">
       <c r="A2" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="2">
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22.5">
+    <row r="3" spans="1:3" ht="23">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>104</v>
       </c>
-      <c r="C3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="22.5">
+    <row r="4" spans="1:3" ht="23">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>105</v>
       </c>
-      <c r="C4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2">
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="22.5">
+    <row r="5" spans="1:3" ht="23">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>106</v>
       </c>
-      <c r="C5" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2">
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="22.5">
+    <row r="6" spans="1:3" ht="23">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>107</v>
       </c>
-      <c r="C6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="2">
         <v>13.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="22.5">
+    <row r="7" spans="1:3" ht="23">
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B7" t="s">
         <v>108</v>
       </c>
-      <c r="C7" t="s">
-        <v>160</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="2">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="22.5">
+    <row r="8" spans="1:3" ht="23">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>109</v>
       </c>
-      <c r="C8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" s="2">
         <v>15.4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.5">
+    <row r="9" spans="1:3" ht="23">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>110</v>
       </c>
-      <c r="C9" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" s="2">
         <v>12.4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.5">
+    <row r="10" spans="1:3" ht="23">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B10" t="s">
         <v>153</v>
       </c>
-      <c r="C10" t="s">
-        <v>163</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.5">
+    <row r="11" spans="1:3" ht="23">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B11" t="s">
         <v>111</v>
       </c>
-      <c r="C11" t="s">
-        <v>164</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="C11" s="2">
         <v>9.1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="22.5">
+    <row r="12" spans="1:3" ht="23">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>112</v>
       </c>
-      <c r="C12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="2">
         <v>8.9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.5">
+    <row r="13" spans="1:3" ht="23">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>113</v>
       </c>
-      <c r="C13" t="s">
-        <v>166</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C13" s="2">
         <v>14.1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="22.5">
+    <row r="14" spans="1:3" ht="23">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>114</v>
       </c>
-      <c r="C14" t="s">
-        <v>167</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C14" s="2">
         <v>10.7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="22.5">
+    <row r="15" spans="1:3" ht="23">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B15" t="s">
         <v>115</v>
       </c>
-      <c r="C15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="C15" s="2">
         <v>12.9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="22.5">
+    <row r="16" spans="1:3" ht="23">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B16" t="s">
         <v>116</v>
       </c>
-      <c r="C16" t="s">
-        <v>169</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="C16" s="2">
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="22.5">
+    <row r="17" spans="1:3" ht="23">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>117</v>
       </c>
-      <c r="C17" t="s">
-        <v>170</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C17" s="2">
         <v>11.2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="22.5">
+    <row r="18" spans="1:3" ht="23">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B18" t="s">
         <v>118</v>
       </c>
-      <c r="C18" t="s">
-        <v>171</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="C18" s="2">
         <v>11.2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="22.5">
+    <row r="19" spans="1:3" ht="23">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>119</v>
       </c>
-      <c r="C19" t="s">
-        <v>172</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="C19" s="2">
         <v>9.6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="22.5">
+    <row r="20" spans="1:3" ht="23">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" t="s">
         <v>120</v>
       </c>
-      <c r="C20" t="s">
-        <v>173</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="C20" s="2">
         <v>9.1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="22.5">
+    <row r="21" spans="1:3" ht="23">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B21" t="s">
         <v>121</v>
       </c>
-      <c r="C21" t="s">
-        <v>174</v>
-      </c>
-      <c r="D21" s="2">
+      <c r="C21" s="2">
         <v>12.4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="22.5">
+    <row r="22" spans="1:3" ht="23">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>122</v>
       </c>
-      <c r="C22" t="s">
-        <v>175</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="C22" s="2">
         <v>11.3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="22.5">
+    <row r="23" spans="1:3" ht="23">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B23" t="s">
         <v>123</v>
       </c>
-      <c r="C23" t="s">
-        <v>176</v>
-      </c>
-      <c r="D23" s="2">
+      <c r="C23" s="2">
         <v>11.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="22.5">
+    <row r="24" spans="1:3" ht="23">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>124</v>
       </c>
-      <c r="C24" t="s">
-        <v>177</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="C24" s="2">
         <v>8.6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="22.5">
+    <row r="25" spans="1:3" ht="23">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B25" t="s">
         <v>125</v>
       </c>
-      <c r="C25" t="s">
-        <v>178</v>
-      </c>
-      <c r="D25" s="2">
+      <c r="C25" s="2">
         <v>12.1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="22.5">
+    <row r="26" spans="1:3" ht="23">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B26" t="s">
         <v>126</v>
       </c>
-      <c r="C26" t="s">
-        <v>179</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="C26" s="2">
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="22.5">
+    <row r="27" spans="1:3" ht="23">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B27" t="s">
         <v>127</v>
       </c>
-      <c r="C27" t="s">
-        <v>180</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="C27" s="2">
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="22.5">
+    <row r="28" spans="1:3" ht="23">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B28" t="s">
         <v>128</v>
       </c>
-      <c r="C28" t="s">
-        <v>181</v>
-      </c>
-      <c r="D28" s="2">
+      <c r="C28" s="2">
         <v>10.5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="22.5">
+    <row r="29" spans="1:3" ht="23">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B29" t="s">
         <v>129</v>
       </c>
-      <c r="C29" t="s">
-        <v>182</v>
-      </c>
-      <c r="D29" s="2">
+      <c r="C29" s="2">
         <v>11.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="22.5">
+    <row r="30" spans="1:3" ht="23">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
         <v>130</v>
       </c>
-      <c r="C30" t="s">
-        <v>183</v>
-      </c>
-      <c r="D30" s="2">
+      <c r="C30" s="2">
         <v>9.6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="22.5">
+    <row r="31" spans="1:3" ht="23">
       <c r="A31" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B31" t="s">
         <v>131</v>
       </c>
-      <c r="C31" t="s">
-        <v>184</v>
-      </c>
-      <c r="D31" s="2">
+      <c r="C31" s="2">
         <v>9.6</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="22.5">
+    <row r="32" spans="1:3" ht="23">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B32" t="s">
         <v>132</v>
       </c>
-      <c r="C32" t="s">
-        <v>185</v>
-      </c>
-      <c r="D32" s="2">
+      <c r="C32" s="2">
         <v>13.2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="22.5">
+    <row r="33" spans="1:3" ht="23">
       <c r="A33" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B33" t="s">
         <v>133</v>
       </c>
-      <c r="C33" t="s">
-        <v>186</v>
-      </c>
-      <c r="D33" s="2">
+      <c r="C33" s="2">
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="22.5">
+    <row r="34" spans="1:3" ht="23">
       <c r="A34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B34" t="s">
         <v>134</v>
       </c>
-      <c r="C34" t="s">
-        <v>187</v>
-      </c>
-      <c r="D34" s="2">
+      <c r="C34" s="2">
         <v>15.9</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="22.5">
+    <row r="35" spans="1:3" ht="23">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>135</v>
       </c>
-      <c r="C35" t="s">
-        <v>188</v>
-      </c>
-      <c r="D35" s="2">
+      <c r="C35" s="2">
         <v>9.9</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="22.5">
+    <row r="36" spans="1:3" ht="23">
       <c r="A36" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B36" t="s">
         <v>136</v>
       </c>
-      <c r="C36" t="s">
-        <v>189</v>
-      </c>
-      <c r="D36" s="2">
+      <c r="C36" s="2">
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="22.5">
+    <row r="37" spans="1:3" ht="23">
       <c r="A37" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B37" t="s">
         <v>137</v>
       </c>
-      <c r="C37" t="s">
-        <v>190</v>
-      </c>
-      <c r="D37" s="2">
+      <c r="C37" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="22.5">
+    <row r="38" spans="1:3" ht="23">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>138</v>
       </c>
-      <c r="C38" t="s">
-        <v>191</v>
-      </c>
-      <c r="D38" s="2">
+      <c r="C38" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="22.5">
+    <row r="39" spans="1:3" ht="23">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B39" t="s">
         <v>139</v>
       </c>
-      <c r="C39" t="s">
-        <v>192</v>
-      </c>
-      <c r="D39" s="2">
+      <c r="C39" s="2">
         <v>10.8</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="22.5">
+    <row r="40" spans="1:3" ht="23">
       <c r="A40" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B40" t="s">
         <v>140</v>
       </c>
-      <c r="C40" t="s">
-        <v>193</v>
-      </c>
-      <c r="D40" s="2">
+      <c r="C40" s="2">
         <v>10.6</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="22.5">
+    <row r="41" spans="1:3" ht="23">
       <c r="A41" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B41" t="s">
         <v>141</v>
       </c>
-      <c r="C41" t="s">
-        <v>194</v>
-      </c>
-      <c r="D41" s="2">
+      <c r="C41" s="2">
         <v>11.4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="22.5">
+    <row r="42" spans="1:3" ht="23">
       <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>142</v>
       </c>
-      <c r="C42" t="s">
-        <v>195</v>
-      </c>
-      <c r="D42" s="2">
+      <c r="C42" s="2">
         <v>8.9</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="22.5">
+    <row r="43" spans="1:3" ht="23">
       <c r="A43" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B43" t="s">
         <v>143</v>
       </c>
-      <c r="C43" t="s">
-        <v>196</v>
-      </c>
-      <c r="D43" s="2">
+      <c r="C43" s="2">
         <v>8.4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="22.5">
+    <row r="44" spans="1:3" ht="23">
       <c r="A44" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B44" t="s">
         <v>144</v>
       </c>
-      <c r="C44" t="s">
-        <v>197</v>
-      </c>
-      <c r="D44" s="2">
+      <c r="C44" s="2">
         <v>7.6</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="22.5">
+    <row r="45" spans="1:3" ht="23">
       <c r="A45" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B45" t="s">
         <v>145</v>
       </c>
-      <c r="C45" t="s">
-        <v>198</v>
-      </c>
-      <c r="D45" s="2">
+      <c r="C45" s="2">
         <v>8.6</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="22.5">
+    <row r="46" spans="1:3" ht="23">
       <c r="A46" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B46" t="s">
         <v>146</v>
       </c>
-      <c r="C46" t="s">
-        <v>199</v>
-      </c>
-      <c r="D46" s="2">
+      <c r="C46" s="2">
         <v>12.1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="22.5">
+    <row r="47" spans="1:3" ht="23">
       <c r="A47" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B47" t="s">
         <v>147</v>
       </c>
-      <c r="C47" t="s">
-        <v>200</v>
-      </c>
-      <c r="D47" s="2">
+      <c r="C47" s="2">
         <v>13.6</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="22.5">
+    <row r="48" spans="1:3" ht="23">
       <c r="A48" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B48" t="s">
         <v>148</v>
       </c>
-      <c r="C48" t="s">
-        <v>201</v>
-      </c>
-      <c r="D48" s="2">
+      <c r="C48" s="2">
         <v>12.5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="22.5">
+    <row r="49" spans="1:3" ht="23">
       <c r="A49" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B49" t="s">
         <v>149</v>
       </c>
-      <c r="C49" t="s">
-        <v>202</v>
-      </c>
-      <c r="D49" s="2">
+      <c r="C49" s="2">
         <v>10.7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="22.5">
+    <row r="50" spans="1:3" ht="23">
       <c r="A50" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B50" t="s">
         <v>150</v>
       </c>
-      <c r="C50" t="s">
-        <v>203</v>
-      </c>
-      <c r="D50" s="2">
+      <c r="C50" s="2">
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="22.5">
+    <row r="51" spans="1:3" ht="23">
       <c r="A51" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B51" t="s">
         <v>151</v>
       </c>
-      <c r="C51" t="s">
-        <v>204</v>
-      </c>
-      <c r="D51" s="2">
+      <c r="C51" s="2">
         <v>10.9</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="22.5">
+    <row r="52" spans="1:3" ht="23">
       <c r="A52" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B52" t="s">
         <v>152</v>
       </c>
-      <c r="C52" t="s">
-        <v>205</v>
-      </c>
-      <c r="D52" s="2">
+      <c r="C52" s="2">
         <v>7.5</v>
       </c>
     </row>
@@ -1774,9 +1462,9 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>